<commit_message>
updated orcad bom from current master bom.
</commit_message>
<xml_diff>
--- a/board/bom2.xlsx
+++ b/board/bom2.xlsx
@@ -10,12 +10,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="331">
   <si>
     <t>Item Number</t>
   </si>
@@ -977,97 +976,37 @@
     <t>Panasonic</t>
   </si>
   <si>
-    <t>0604</t>
-  </si>
-  <si>
-    <t>0605</t>
-  </si>
-  <si>
-    <t>0606</t>
-  </si>
-  <si>
-    <t>0607</t>
-  </si>
-  <si>
-    <t>0608</t>
-  </si>
-  <si>
-    <t>0609</t>
-  </si>
-  <si>
-    <t>0610</t>
-  </si>
-  <si>
-    <t>0611</t>
-  </si>
-  <si>
-    <t>0612</t>
-  </si>
-  <si>
-    <t>0613</t>
-  </si>
-  <si>
-    <t>0614</t>
-  </si>
-  <si>
-    <t>0615</t>
-  </si>
-  <si>
-    <t>0616</t>
-  </si>
-  <si>
-    <t>0617</t>
-  </si>
-  <si>
-    <t>0618</t>
-  </si>
-  <si>
-    <t>0619</t>
-  </si>
-  <si>
-    <t>0620</t>
-  </si>
-  <si>
-    <t>0621</t>
-  </si>
-  <si>
-    <t>0622</t>
-  </si>
-  <si>
-    <t>0623</t>
-  </si>
-  <si>
-    <t>0624</t>
-  </si>
-  <si>
-    <t>0625</t>
-  </si>
-  <si>
-    <t>0626</t>
-  </si>
-  <si>
-    <t>0627</t>
-  </si>
-  <si>
-    <t>0628</t>
-  </si>
-  <si>
-    <t>0629</t>
-  </si>
-  <si>
-    <t>0630</t>
-  </si>
-  <si>
-    <t>0631</t>
-  </si>
-  <si>
-    <t>0632</t>
-  </si>
-  <si>
-    <t>0633</t>
-  </si>
-  <si>
-    <t>0634</t>
+    <t>P2.00KHCT-ND</t>
+  </si>
+  <si>
+    <t>H12193CT-ND</t>
+  </si>
+  <si>
+    <t>FTDI</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>490-9716-1-ND</t>
+  </si>
+  <si>
+    <t>F2594CT-ND</t>
+  </si>
+  <si>
+    <t>Littlefuse</t>
+  </si>
+  <si>
+    <t>PLTT20.0KACT-ND</t>
+  </si>
+  <si>
+    <t>PLTT50.0KACT-ND</t>
+  </si>
+  <si>
+    <t>PLTT499ACT-ND</t>
+  </si>
+  <si>
+    <t>Vishay</t>
   </si>
 </sst>
 </file>
@@ -1415,8 +1354,8 @@
   <dimension ref="A1:I204"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E111" sqref="E111"/>
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E151" sqref="E151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3743,13 +3682,13 @@
         <v>318</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>320</v>
+        <v>17</v>
       </c>
       <c r="H80" t="s">
         <v>319</v>
       </c>
       <c r="I80">
-        <v>1.1000000000000001</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3772,13 +3711,13 @@
         <v>318</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>321</v>
+        <v>17</v>
       </c>
       <c r="H81" t="s">
         <v>319</v>
       </c>
       <c r="I81">
-        <v>2.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -3801,13 +3740,13 @@
         <v>318</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>322</v>
+        <v>17</v>
       </c>
       <c r="H82" t="s">
         <v>319</v>
       </c>
       <c r="I82">
-        <v>3.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -3830,13 +3769,13 @@
         <v>318</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>323</v>
+        <v>17</v>
       </c>
       <c r="H83" t="s">
         <v>319</v>
       </c>
       <c r="I83">
-        <v>4.0999999999999996</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -3859,13 +3798,13 @@
         <v>318</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>324</v>
+        <v>17</v>
       </c>
       <c r="H84" t="s">
         <v>319</v>
       </c>
       <c r="I84">
-        <v>5.0999999999999996</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -3888,13 +3827,13 @@
         <v>318</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>325</v>
+        <v>17</v>
       </c>
       <c r="H85" t="s">
         <v>319</v>
       </c>
       <c r="I85">
-        <v>6.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -3917,13 +3856,13 @@
         <v>318</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>326</v>
+        <v>17</v>
       </c>
       <c r="H86" t="s">
         <v>319</v>
       </c>
       <c r="I86">
-        <v>7.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -3946,13 +3885,13 @@
         <v>318</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>327</v>
+        <v>17</v>
       </c>
       <c r="H87" t="s">
         <v>319</v>
       </c>
       <c r="I87">
-        <v>8.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -3975,13 +3914,13 @@
         <v>318</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>328</v>
+        <v>17</v>
       </c>
       <c r="H88" t="s">
         <v>319</v>
       </c>
       <c r="I88">
-        <v>9.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -4004,13 +3943,13 @@
         <v>318</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>329</v>
+        <v>17</v>
       </c>
       <c r="H89" t="s">
         <v>319</v>
       </c>
       <c r="I89">
-        <v>10.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -4033,13 +3972,13 @@
         <v>318</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>330</v>
+        <v>17</v>
       </c>
       <c r="H90" t="s">
         <v>319</v>
       </c>
       <c r="I90">
-        <v>11.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -4062,13 +4001,13 @@
         <v>318</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>331</v>
+        <v>17</v>
       </c>
       <c r="H91" t="s">
         <v>319</v>
       </c>
       <c r="I91">
-        <v>12.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -4091,13 +4030,13 @@
         <v>318</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>332</v>
+        <v>17</v>
       </c>
       <c r="H92" t="s">
         <v>319</v>
       </c>
       <c r="I92">
-        <v>13.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -4120,13 +4059,13 @@
         <v>318</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>333</v>
+        <v>17</v>
       </c>
       <c r="H93" t="s">
         <v>319</v>
       </c>
       <c r="I93">
-        <v>14.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -4149,13 +4088,13 @@
         <v>318</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>334</v>
+        <v>17</v>
       </c>
       <c r="H94" t="s">
         <v>319</v>
       </c>
       <c r="I94">
-        <v>15.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -4178,13 +4117,13 @@
         <v>318</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>335</v>
+        <v>17</v>
       </c>
       <c r="H95" t="s">
         <v>319</v>
       </c>
       <c r="I95">
-        <v>16.100000000000001</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -4207,13 +4146,13 @@
         <v>318</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>336</v>
+        <v>17</v>
       </c>
       <c r="H96" t="s">
         <v>319</v>
       </c>
       <c r="I96">
-        <v>17.100000000000001</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -4236,13 +4175,13 @@
         <v>318</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>337</v>
+        <v>17</v>
       </c>
       <c r="H97" t="s">
         <v>319</v>
       </c>
       <c r="I97">
-        <v>18.100000000000001</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -4265,13 +4204,13 @@
         <v>318</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>338</v>
+        <v>17</v>
       </c>
       <c r="H98" t="s">
         <v>319</v>
       </c>
       <c r="I98">
-        <v>19.100000000000001</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -4294,13 +4233,13 @@
         <v>318</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>339</v>
+        <v>17</v>
       </c>
       <c r="H99" t="s">
         <v>319</v>
       </c>
       <c r="I99">
-        <v>20.100000000000001</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -4323,13 +4262,13 @@
         <v>318</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>340</v>
+        <v>17</v>
       </c>
       <c r="H100" t="s">
         <v>319</v>
       </c>
       <c r="I100">
-        <v>21.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -4352,13 +4291,13 @@
         <v>318</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>341</v>
+        <v>17</v>
       </c>
       <c r="H101" t="s">
         <v>319</v>
       </c>
       <c r="I101">
-        <v>22.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -4381,13 +4320,13 @@
         <v>318</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>342</v>
+        <v>17</v>
       </c>
       <c r="H102" t="s">
         <v>319</v>
       </c>
       <c r="I102">
-        <v>23.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -4410,13 +4349,13 @@
         <v>318</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>343</v>
+        <v>17</v>
       </c>
       <c r="H103" t="s">
         <v>319</v>
       </c>
       <c r="I103">
-        <v>24.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -4439,13 +4378,13 @@
         <v>318</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>344</v>
+        <v>17</v>
       </c>
       <c r="H104" t="s">
         <v>319</v>
       </c>
       <c r="I104">
-        <v>25.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -4468,13 +4407,13 @@
         <v>318</v>
       </c>
       <c r="G105" s="2" t="s">
-        <v>345</v>
+        <v>17</v>
       </c>
       <c r="H105" t="s">
         <v>319</v>
       </c>
       <c r="I105">
-        <v>26.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -4497,13 +4436,13 @@
         <v>318</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>346</v>
+        <v>17</v>
       </c>
       <c r="H106" t="s">
         <v>319</v>
       </c>
       <c r="I106">
-        <v>27.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -4526,13 +4465,13 @@
         <v>318</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>347</v>
+        <v>17</v>
       </c>
       <c r="H107" t="s">
         <v>319</v>
       </c>
       <c r="I107">
-        <v>28.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -4555,13 +4494,13 @@
         <v>318</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>348</v>
+        <v>17</v>
       </c>
       <c r="H108" t="s">
         <v>319</v>
       </c>
       <c r="I108">
-        <v>29.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -4584,13 +4523,13 @@
         <v>318</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>349</v>
+        <v>17</v>
       </c>
       <c r="H109" t="s">
         <v>319</v>
       </c>
       <c r="I109">
-        <v>30.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -4613,13 +4552,13 @@
         <v>318</v>
       </c>
       <c r="G110" s="2" t="s">
-        <v>350</v>
+        <v>17</v>
       </c>
       <c r="H110" t="s">
         <v>319</v>
       </c>
       <c r="I110">
-        <v>31.1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -4638,17 +4577,17 @@
       <c r="E111" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="F111" s="2" t="s">
-        <v>12</v>
+      <c r="F111" t="s">
+        <v>320</v>
       </c>
       <c r="G111" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I111" s="3" t="s">
-        <v>12</v>
+        <v>319</v>
+      </c>
+      <c r="I111" s="3">
+        <v>0.1</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -4667,17 +4606,17 @@
       <c r="E112" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="F112" s="2" t="s">
-        <v>12</v>
+      <c r="F112" t="s">
+        <v>320</v>
       </c>
       <c r="G112" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I112" s="3" t="s">
-        <v>12</v>
+        <v>319</v>
+      </c>
+      <c r="I112" s="3">
+        <v>0.1</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -4696,17 +4635,17 @@
       <c r="E113" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="F113" s="2" t="s">
-        <v>12</v>
+      <c r="F113" t="s">
+        <v>320</v>
       </c>
       <c r="G113" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I113" s="3" t="s">
-        <v>12</v>
+        <v>319</v>
+      </c>
+      <c r="I113" s="3">
+        <v>0.1</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -4725,17 +4664,17 @@
       <c r="E114" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="F114" s="2" t="s">
-        <v>12</v>
+      <c r="F114" t="s">
+        <v>320</v>
       </c>
       <c r="G114" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I114" s="3" t="s">
-        <v>12</v>
+        <v>319</v>
+      </c>
+      <c r="I114" s="3">
+        <v>0.1</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -4754,17 +4693,17 @@
       <c r="E115" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F115" s="2" t="s">
-        <v>12</v>
+      <c r="F115" t="s">
+        <v>320</v>
       </c>
       <c r="G115" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I115" s="3" t="s">
-        <v>12</v>
+        <v>319</v>
+      </c>
+      <c r="I115" s="3">
+        <v>0.1</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -4783,17 +4722,17 @@
       <c r="E116" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F116" s="2" t="s">
-        <v>12</v>
+      <c r="F116" t="s">
+        <v>320</v>
       </c>
       <c r="G116" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H116" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I116" s="3" t="s">
-        <v>12</v>
+        <v>319</v>
+      </c>
+      <c r="I116" s="3">
+        <v>0.1</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -4812,17 +4751,17 @@
       <c r="E117" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="F117" s="2" t="s">
-        <v>12</v>
+      <c r="F117" t="s">
+        <v>320</v>
       </c>
       <c r="G117" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I117" s="3" t="s">
-        <v>12</v>
+        <v>319</v>
+      </c>
+      <c r="I117" s="3">
+        <v>0.1</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -4841,17 +4780,17 @@
       <c r="E118" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="F118" s="2" t="s">
-        <v>12</v>
+      <c r="F118" t="s">
+        <v>320</v>
       </c>
       <c r="G118" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H118" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I118" s="3" t="s">
-        <v>12</v>
+        <v>319</v>
+      </c>
+      <c r="I118" s="3">
+        <v>0.1</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -4870,17 +4809,17 @@
       <c r="E119" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="F119" s="2" t="s">
-        <v>12</v>
+      <c r="F119" t="s">
+        <v>320</v>
       </c>
       <c r="G119" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H119" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I119" s="3" t="s">
-        <v>12</v>
+        <v>319</v>
+      </c>
+      <c r="I119" s="3">
+        <v>0.1</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -4899,17 +4838,17 @@
       <c r="E120" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="F120" s="2" t="s">
-        <v>12</v>
+      <c r="F120" t="s">
+        <v>321</v>
       </c>
       <c r="G120" s="2" t="s">
         <v>277</v>
       </c>
       <c r="H120" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I120" s="3" t="s">
-        <v>12</v>
+        <v>322</v>
+      </c>
+      <c r="I120">
+        <v>2</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -4928,17 +4867,17 @@
       <c r="E121" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F121" s="2" t="s">
-        <v>12</v>
+      <c r="F121" t="s">
+        <v>324</v>
       </c>
       <c r="G121" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I121" s="3" t="s">
-        <v>12</v>
+        <v>323</v>
+      </c>
+      <c r="I121">
+        <v>0.16</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -4958,16 +4897,16 @@
         <v>38</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>12</v>
+        <v>324</v>
       </c>
       <c r="G122" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H122" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I122" s="3" t="s">
-        <v>12</v>
+        <v>323</v>
+      </c>
+      <c r="I122" s="3">
+        <v>0.16</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -4987,16 +4926,16 @@
         <v>38</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>12</v>
+        <v>324</v>
       </c>
       <c r="G123" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I123" s="3" t="s">
-        <v>12</v>
+        <v>323</v>
+      </c>
+      <c r="I123" s="3">
+        <v>0.16</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -5016,16 +4955,16 @@
         <v>38</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>12</v>
+        <v>324</v>
       </c>
       <c r="G124" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H124" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I124" s="3" t="s">
-        <v>12</v>
+        <v>323</v>
+      </c>
+      <c r="I124" s="3">
+        <v>0.16</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -5045,16 +4984,16 @@
         <v>48</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>12</v>
+        <v>324</v>
       </c>
       <c r="G125" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I125" s="3" t="s">
-        <v>12</v>
+        <v>323</v>
+      </c>
+      <c r="I125" s="3">
+        <v>0.16</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -5074,16 +5013,16 @@
         <v>48</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>12</v>
+        <v>324</v>
       </c>
       <c r="G126" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H126" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I126" s="3" t="s">
-        <v>12</v>
+        <v>323</v>
+      </c>
+      <c r="I126" s="3">
+        <v>0.16</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -5103,16 +5042,16 @@
         <v>52</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>12</v>
+        <v>324</v>
       </c>
       <c r="G127" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H127" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I127" s="3" t="s">
-        <v>12</v>
+        <v>323</v>
+      </c>
+      <c r="I127" s="3">
+        <v>0.16</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -5132,16 +5071,16 @@
         <v>52</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>12</v>
+        <v>324</v>
       </c>
       <c r="G128" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H128" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I128" s="3" t="s">
-        <v>12</v>
+        <v>323</v>
+      </c>
+      <c r="I128" s="3">
+        <v>0.16</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -5161,16 +5100,16 @@
         <v>52</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>12</v>
+        <v>324</v>
       </c>
       <c r="G129" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H129" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I129" s="3" t="s">
-        <v>12</v>
+        <v>323</v>
+      </c>
+      <c r="I129" s="3">
+        <v>0.16</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -5190,16 +5129,16 @@
         <v>52</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>12</v>
+        <v>324</v>
       </c>
       <c r="G130" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H130" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I130" s="3" t="s">
-        <v>12</v>
+        <v>323</v>
+      </c>
+      <c r="I130" s="3">
+        <v>0.16</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
@@ -5624,17 +5563,17 @@
       <c r="E145" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F145" s="2" t="s">
-        <v>12</v>
+      <c r="F145" t="s">
+        <v>325</v>
       </c>
       <c r="G145" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H145" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I145" s="3" t="s">
-        <v>12</v>
+        <v>326</v>
+      </c>
+      <c r="I145">
+        <v>0.67</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
@@ -5653,17 +5592,17 @@
       <c r="E146" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F146" s="2" t="s">
-        <v>12</v>
+      <c r="F146" t="s">
+        <v>325</v>
       </c>
       <c r="G146" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H146" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I146" s="3" t="s">
-        <v>12</v>
+        <v>326</v>
+      </c>
+      <c r="I146">
+        <v>0.67</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -5682,17 +5621,17 @@
       <c r="E147" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F147" s="2" t="s">
-        <v>12</v>
+      <c r="F147" t="s">
+        <v>327</v>
       </c>
       <c r="G147" s="2" t="s">
         <v>237</v>
       </c>
       <c r="H147" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I147" s="3" t="s">
-        <v>12</v>
+        <v>330</v>
+      </c>
+      <c r="I147">
+        <v>11.25</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
@@ -5711,17 +5650,17 @@
       <c r="E148" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="F148" s="2" t="s">
-        <v>12</v>
+      <c r="F148" t="s">
+        <v>329</v>
       </c>
       <c r="G148" s="2" t="s">
         <v>237</v>
       </c>
       <c r="H148" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I148" s="3" t="s">
-        <v>12</v>
+        <v>330</v>
+      </c>
+      <c r="I148">
+        <v>11.25</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -5740,17 +5679,17 @@
       <c r="E149" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="F149" s="2" t="s">
-        <v>12</v>
+      <c r="F149" t="s">
+        <v>328</v>
       </c>
       <c r="G149" s="2" t="s">
         <v>237</v>
       </c>
       <c r="H149" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I149" s="3" t="s">
-        <v>12</v>
+        <v>330</v>
+      </c>
+      <c r="I149">
+        <v>11.25</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
@@ -5768,9 +5707,6 @@
       </c>
       <c r="E150" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="F150" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="G150" s="2" t="s">
         <v>17</v>

</xml_diff>